<commit_message>
refactor: sample dataset that demonstrate all cleaning operations
</commit_message>
<xml_diff>
--- a/examples/rawData/sample_dataset_dict.xlsx
+++ b/examples/rawData/sample_dataset_dict.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kwokjh\Documents\repo\copula-tabular\examples\rawData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kwokjh\Documents\repo\copular-tabular-fork\examples\rawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79AC5EBB-57A0-458A-BA9E-E5EDB65519F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B8897A-A4D5-4E48-8A06-C63F970B4F91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="58">
   <si>
     <t>NAME</t>
   </si>
@@ -60,9 +60,6 @@
   </si>
   <si>
     <t>CONSTRAINTS</t>
-  </si>
-  <si>
-    <t>ID</t>
   </si>
   <si>
     <t>date</t>
@@ -192,15 +189,37 @@
   </si>
   <si>
     <t>Body mass index category. Reported for participants aged 2 years or older. One of 12.0_18.5, 18.5_to_24.9, 25.0_to_29.9, or 30.0_plus.</t>
-  </si>
-  <si>
-    <t>12.0_18.4; 18.5_24.9; 25.0_29.9; 30.0_plus</t>
   </si>
   <si>
     <t>a) If 'bmi' &lt;=18.4, =&gt; 'BMI_WHO' = '12.0_18.5'
 b) If 'bmi' &lt;=24.9, =&gt; 'BMI_WHO' = '18.5_24.9'
 c) If 'bmi' &lt;=29.9, =&gt; 'BMI_WHO' = '25.0_29.9'
 d) Else =&gt; 'BMI_WHO' = '30.0_plus'</t>
+  </si>
+  <si>
+    <t>ROWID</t>
+  </si>
+  <si>
+    <t>Total Care Cost</t>
+  </si>
+  <si>
+    <t>PID</t>
+  </si>
+  <si>
+    <t>12.0_18.5; 18.5_to_24.9; 25.0_to_29.9; 30.0_plus</t>
+  </si>
+  <si>
+    <t>Total care cost of participant.
+To test the exclusion list of the Character Conversion operation</t>
+  </si>
+  <si>
+    <t>Financial Information</t>
+  </si>
+  <si>
+    <t>[0,150]</t>
+  </si>
+  <si>
+    <t>[0,200]</t>
   </si>
 </sst>
 </file>
@@ -265,7 +284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -281,6 +300,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -562,17 +590,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="96" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.5703125" customWidth="1"/>
     <col min="2" max="2" width="32.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="46" customWidth="1"/>
     <col min="5" max="5" width="25.140625" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
@@ -605,32 +633,33 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="2" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6" t="s">
         <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>25</v>
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -638,212 +667,214 @@
     </row>
     <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>39</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5">
         <v>4</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6">
         <v>5</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="2" t="s">
+    </row>
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="F7">
         <v>6</v>
       </c>
+      <c r="G7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>57</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="2"/>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
       <c r="E9" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F9">
         <v>8</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F10">
         <v>9</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F11">
         <v>10</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" t="s">
-        <v>9</v>
+        <v>22</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F12">
         <v>11</v>
       </c>
+      <c r="G12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="13" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F13">
         <v>12</v>
@@ -851,16 +882,19 @@
     </row>
     <row r="14" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>12</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F14">
         <v>13</v>
@@ -868,29 +902,61 @@
     </row>
     <row r="15" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E16" s="2"/>
+    <row r="16" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>